<commit_message>
Adding test case group for Search Verification
</commit_message>
<xml_diff>
--- a/KaiKaci_Manual_Test_Cases.xlsx
+++ b/KaiKaci_Manual_Test_Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\FinalSoftware\KIU_Volunteer_Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30A9DC5D-44B1-45D7-851D-DAF40740BBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610AEAFA-97BD-46BA-9738-E3577E8EFF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8D77261-4695-4176-9C21-633C78935755}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -179,12 +179,106 @@
   <si>
     <t>TC_01</t>
   </si>
+  <si>
+    <t>TC_02_01</t>
+  </si>
+  <si>
+    <t>Search by full title returns matching events</t>
+  </si>
+  <si>
+    <t>Tester is on the landing page. At least two events exist, including one titled 'Beach Cleanup'.</t>
+  </si>
+  <si>
+    <t>1. Locate the search input in the nav bar.
+2. Type 'Beach Cleanup'.
+3. Click the search icon.</t>
+  </si>
+  <si>
+    <t>TC_02_02</t>
+  </si>
+  <si>
+    <t>Search is case‑insensitive</t>
+  </si>
+  <si>
+    <t>Tester is on the landing page with at least one event titled 'Tree Planting'.</t>
+  </si>
+  <si>
+    <t>1. Clear any existing search term.
+2. Type 'tree planting' in lowercase.
+3. Click the search icon.</t>
+  </si>
+  <si>
+    <t>TC_02_03</t>
+  </si>
+  <si>
+    <t>Search with no matches displays 'No events found' message</t>
+  </si>
+  <si>
+    <t>Tester is on the landing page.</t>
+  </si>
+  <si>
+    <t>1. Clear the search field.
+2. Type 'qwerty123'.
+3. Click the search icon.</t>
+  </si>
+  <si>
+    <t>TC_02_04</t>
+  </si>
+  <si>
+    <t>Clearing search restores full event list</t>
+  </si>
+  <si>
+    <t>Search results are currently filtered (e.g., after running TC_02_01).</t>
+  </si>
+  <si>
+    <t>1. Clear the text in the search field.
+2. Click the search icon or press Enter.</t>
+  </si>
+  <si>
+    <t>TC_02_05</t>
+  </si>
+  <si>
+    <t>Match count updates live as user types</t>
+  </si>
+  <si>
+    <t>Tester is on the landing page. At least three events exist with distinct titles.</t>
+  </si>
+  <si>
+    <t>1. Focus the search input.
+2. Type 'Be'.
+3. Observe the match count dropdown/label.
+4. Continue typing to 'Bea'.</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>KaiKaci Search Test Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Only the 'Beach Cleanup' event card is displayed in the grid. 
+2. The match count shows </t>
+  </si>
+  <si>
+    <t>1. The 'Tree Planting' event appears despite case differences.
+2. Match count reflects the correct number of results.</t>
+  </si>
+  <si>
+    <t>1. Event grid is hidden or empty and a 'No events found' banner/message is shown.
+2. Match count shows 0.</t>
+  </si>
+  <si>
+    <t>1. All events are displayed again and match count equals total events.</t>
+  </si>
+  <si>
+    <t>1. Match count updates in real‑time reflecting the number of events containing the current text fragment.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +318,19 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -298,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -325,6 +432,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,19 +775,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85E657A-BF65-4825-A55E-19D5A6F59D35}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="25.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -683,8 +799,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" outlineLevel="1"/>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="2" spans="1:7" outlineLevel="1"/>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -704,7 +820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="206.25" customHeight="1" outlineLevel="1">
+    <row r="4" spans="1:7" ht="206.25" customHeight="1" outlineLevel="1">
       <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
@@ -724,7 +840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" outlineLevel="1">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" outlineLevel="1">
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -732,7 +848,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -752,7 +868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="128.25" outlineLevel="1">
+    <row r="7" spans="1:7" ht="156.75" outlineLevel="1">
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
@@ -772,7 +888,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="15" outlineLevel="1">
+    <row r="8" spans="1:7" ht="15" outlineLevel="1">
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -780,7 +896,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B9" s="8" t="s">
         <v>0</v>
       </c>
@@ -800,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="99.75" outlineLevel="1">
+    <row r="10" spans="1:7" ht="114" outlineLevel="1">
       <c r="B10" s="4" t="s">
         <v>35</v>
       </c>
@@ -820,7 +936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="15" outlineLevel="1">
+    <row r="11" spans="1:7" ht="15" outlineLevel="1">
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -828,7 +944,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -848,7 +964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="114" outlineLevel="1">
+    <row r="13" spans="1:7" ht="128.25" outlineLevel="1">
       <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
@@ -868,7 +984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="15" outlineLevel="1">
+    <row r="14" spans="1:7" ht="15" outlineLevel="1">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -876,7 +992,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B15" s="8" t="s">
         <v>0</v>
       </c>
@@ -896,7 +1012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="71.25" outlineLevel="1">
+    <row r="16" spans="1:7" ht="85.5" outlineLevel="1">
       <c r="B16" s="4" t="s">
         <v>37</v>
       </c>
@@ -916,7 +1032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:7" s="1" customFormat="1" ht="15" outlineLevel="1">
+    <row r="17" spans="1:7" ht="15" outlineLevel="1">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -924,7 +1040,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" s="1" customFormat="1" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B18" s="8" t="s">
         <v>0</v>
       </c>
@@ -944,7 +1060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:7" s="1" customFormat="1" ht="85.5" outlineLevel="1">
+    <row r="19" spans="1:7" ht="99.75" outlineLevel="1">
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
@@ -964,8 +1080,251 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:7" outlineLevel="1"/>
-    <row r="21" spans="2:7" outlineLevel="1"/>
+    <row r="20" spans="1:7" outlineLevel="1"/>
+    <row r="21" spans="1:7" outlineLevel="1"/>
+    <row r="23" spans="1:7" s="11" customFormat="1" ht="15.75">
+      <c r="A23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" outlineLevel="1"/>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B25" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="90" outlineLevel="1">
+      <c r="B26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="75" outlineLevel="1">
+      <c r="B29" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B31" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="75" outlineLevel="1">
+      <c r="B32" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B34" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="60" outlineLevel="1">
+      <c r="B35" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+    </row>
+    <row r="37" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B37" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="75" outlineLevel="1">
+      <c r="B38" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" outlineLevel="1"/>
+    <row r="40" spans="2:7" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding test case group for Event test cases
</commit_message>
<xml_diff>
--- a/KaiKaci_Manual_Test_Cases.xlsx
+++ b/KaiKaci_Manual_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\FinalSoftware\KIU_Volunteer_Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2769996F-6394-4FCD-8138-EFE298CCA67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE54011-B1AF-441C-B044-4B2BA4F5D40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="122">
   <si>
     <t>TC_01</t>
   </si>
@@ -373,12 +373,112 @@
 2. 'Login / Register' button returns to nav bar.
 3. Any authenticated-only pages are no longer accessible without login.</t>
   </si>
+  <si>
+    <t>TC_04_01</t>
+  </si>
+  <si>
+    <t>Event page loads with hero image and details</t>
+  </si>
+  <si>
+    <t>Tester is on the landing page. At least one event exists and is open.</t>
+  </si>
+  <si>
+    <t>1. Click any open event card.
+2. Observe the event page elements.</t>
+  </si>
+  <si>
+    <t>1. Event page loads successfully.
+2. Hero image is visible (or placeholder if no image supplied).
+3. Title, date, location, and description are displayed.
+4. 'Register as Volunteer' button is present and enabled.</t>
+  </si>
+  <si>
+    <t>TC_04_02</t>
+  </si>
+  <si>
+    <t>Logged‑in user registers successfully</t>
+  </si>
+  <si>
+    <t>Tester is logged in and on an event page with open status.</t>
+  </si>
+  <si>
+    <t>1. Click 'Register as Volunteer'.
+2. Modal with open‑text questions appears.
+3. Enter valid answers in all fields.
+4. Click 'Submit'.</t>
+  </si>
+  <si>
+    <t>1. Submission succeeds; modal closes.
+2. Success banner or toast confirms registration.
+3. 'Register as Volunteer' button becomes disabled or changes to 'Pending'.</t>
+  </si>
+  <si>
+    <t>TC_04_03</t>
+  </si>
+  <si>
+    <t>Guest registration prompts login / register flow</t>
+  </si>
+  <si>
+    <t>Tester is NOT logged in and on an event page with open status.</t>
+  </si>
+  <si>
+    <t>1. Click 'Register as Volunteer'.</t>
+  </si>
+  <si>
+    <t>1. Login/Register modal appears instead of the question form.
+2. After successful login/registration, the question form is shown automatically.
+3. User can complete registration as in TC_04_02.</t>
+  </si>
+  <si>
+    <t>TC_04_04</t>
+  </si>
+  <si>
+    <t>Registration form validates empty answers</t>
+  </si>
+  <si>
+    <t>Tester is logged in and on an event page.</t>
+  </si>
+  <si>
+    <t>1. Click 'Register as Volunteer'.
+2. Leave all question fields blank.
+3. Click 'Submit'.</t>
+  </si>
+  <si>
+    <t>1. Form is not submitted.
+2. Inline validation messages appear under each empty field (e.g., 'Answer required').
+3. Submit button remains disabled or re‑enabled once all fields are filled.</t>
+  </si>
+  <si>
+    <t>TC_04_05</t>
+  </si>
+  <si>
+    <t>Duplicate registration is prevented</t>
+  </si>
+  <si>
+    <t>Tester is logged in, has already registered for this event (status = Pending/Accepted).</t>
+  </si>
+  <si>
+    <t>1. Refresh the event page.
+2. Observe the registration section.
+3. Attempt to click 'Register as Volunteer' again.</t>
+  </si>
+  <si>
+    <t>1. Register button is hidden, disabled, or replaced with status badge ('Pending', 'Accepted').
+2. No second submission is allowed.
+3. No duplicate entry is created in the backend.</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>KaiKaci Event Test Cases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +548,33 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -524,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -572,6 +699,38 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -935,7 +1094,7 @@
       <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="22" t="s">
         <v>13</v>
       </c>
     </row>
@@ -945,7 +1104,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B6" s="9" t="s">
@@ -963,7 +1122,7 @@
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -983,7 +1142,7 @@
       <c r="F7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -993,7 +1152,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B9" s="10" t="s">
@@ -1011,7 +1170,7 @@
       <c r="F9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1031,7 +1190,7 @@
       <c r="F10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1041,7 +1200,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B12" s="10" t="s">
@@ -1059,7 +1218,7 @@
       <c r="F12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1079,7 +1238,7 @@
       <c r="F13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1089,7 +1248,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B15" s="10" t="s">
@@ -1107,7 +1266,7 @@
       <c r="F15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1127,7 +1286,7 @@
       <c r="F16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1137,7 +1296,7 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B18" s="10" t="s">
@@ -1155,7 +1314,7 @@
       <c r="F18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1175,12 +1334,19 @@
       <c r="F19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" outlineLevel="1"/>
-    <row r="21" spans="1:7" outlineLevel="1"/>
+    <row r="20" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="1:7" ht="15">
+      <c r="G22" s="26"/>
+    </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75">
       <c r="A23" s="3" t="s">
         <v>41</v>
@@ -1188,8 +1354,11 @@
       <c r="B23" s="18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" outlineLevel="1"/>
+      <c r="G23" s="27"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G24" s="26"/>
+    </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B25" s="10" t="s">
         <v>2</v>
@@ -1206,7 +1375,7 @@
       <c r="F25" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1226,7 +1395,7 @@
       <c r="F26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1236,7 +1405,7 @@
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B28" s="10" t="s">
@@ -1254,7 +1423,7 @@
       <c r="F28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1274,7 +1443,7 @@
       <c r="F29" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1284,7 +1453,7 @@
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B31" s="10" t="s">
@@ -1302,7 +1471,7 @@
       <c r="F31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1322,7 +1491,7 @@
       <c r="F32" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1332,7 +1501,7 @@
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B34" s="10" t="s">
@@ -1350,7 +1519,7 @@
       <c r="F34" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1370,7 +1539,7 @@
       <c r="F35" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1380,7 +1549,7 @@
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B37" s="10" t="s">
@@ -1398,7 +1567,7 @@
       <c r="F37" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1418,12 +1587,19 @@
       <c r="F38" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:7" outlineLevel="1"/>
-    <row r="40" spans="1:7" outlineLevel="1"/>
+    <row r="39" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G39" s="26"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G40" s="26"/>
+    </row>
+    <row r="41" spans="1:7" ht="15">
+      <c r="G41" s="26"/>
+    </row>
     <row r="42" spans="1:7" s="1" customFormat="1" ht="15.75">
       <c r="A42" s="3" t="s">
         <v>68</v>
@@ -1431,8 +1607,11 @@
       <c r="B42" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" outlineLevel="1"/>
+      <c r="G42" s="27"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G43" s="26"/>
+    </row>
     <row r="44" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B44" s="10" t="s">
         <v>2</v>
@@ -1449,7 +1628,7 @@
       <c r="F44" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1469,17 +1648,17 @@
       <c r="F45" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G45" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:7" outlineLevel="1">
+    <row r="46" spans="1:7" ht="15" outlineLevel="1">
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
+      <c r="G46" s="29"/>
     </row>
     <row r="47" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B47" s="10" t="s">
@@ -1497,7 +1676,7 @@
       <c r="F47" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="10" t="s">
+      <c r="G47" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1517,19 +1696,19 @@
       <c r="F48" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="2:7" outlineLevel="1">
+    <row r="49" spans="1:7" ht="15" outlineLevel="1">
       <c r="B49" s="16"/>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-    </row>
-    <row r="50" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="G49" s="29"/>
+    </row>
+    <row r="50" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B50" s="10" t="s">
         <v>2</v>
       </c>
@@ -1545,39 +1724,39 @@
       <c r="F50" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="99.75" outlineLevel="1">
+    <row r="51" spans="1:7" ht="99.75" outlineLevel="1">
       <c r="B51" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E51" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G51" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="2:7" outlineLevel="1">
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-    </row>
-    <row r="53" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="52" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="30"/>
+    </row>
+    <row r="53" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B53" s="10" t="s">
         <v>2</v>
       </c>
@@ -1593,39 +1772,39 @@
       <c r="F53" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G53" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="85.5" outlineLevel="1">
+    <row r="54" spans="1:7" ht="85.5" outlineLevel="1">
       <c r="B54" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="G54" s="15" t="s">
+      <c r="G54" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="2:7" outlineLevel="1">
+    <row r="55" spans="1:7" ht="15" outlineLevel="1">
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
       <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-    </row>
-    <row r="56" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="G55" s="29"/>
+    </row>
+    <row r="56" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B56" s="10" t="s">
         <v>2</v>
       </c>
@@ -1641,31 +1820,285 @@
       <c r="F56" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="G56" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="99.75" outlineLevel="1">
+    <row r="57" spans="1:7" ht="99.75" outlineLevel="1">
       <c r="B57" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="15" t="s">
+      <c r="E57" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F57" s="15" t="s">
+      <c r="F57" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G57" s="15" t="s">
+      <c r="G57" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="2:7" outlineLevel="1"/>
+    <row r="58" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G58" s="26"/>
+    </row>
+    <row r="59" spans="1:7" ht="15">
+      <c r="G59" s="26"/>
+    </row>
+    <row r="60" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A60" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G60" s="27"/>
+    </row>
+    <row r="61" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G61" s="26"/>
+    </row>
+    <row r="62" spans="1:7" ht="15" outlineLevel="1">
+      <c r="G62" s="26"/>
+    </row>
+    <row r="63" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B63" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="128.25" outlineLevel="1">
+      <c r="B64" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G64" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="23"/>
+    </row>
+    <row r="66" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B66" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="99.75" outlineLevel="1">
+      <c r="B67" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="23"/>
+    </row>
+    <row r="69" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B69" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="114" outlineLevel="1">
+      <c r="B70" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="23"/>
+    </row>
+    <row r="72" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B72" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="99.75" outlineLevel="1">
+      <c r="B73" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E73" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G73" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="23"/>
+    </row>
+    <row r="75" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B75" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="114" outlineLevel="1">
+      <c r="B76" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F76" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G76" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" outlineLevel="1"/>
+    <row r="78" spans="2:7" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Adding test case group for Event Create/Edit test cases
</commit_message>
<xml_diff>
--- a/KaiKaci_Manual_Test_Cases.xlsx
+++ b/KaiKaci_Manual_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\FinalSoftware\KIU_Volunteer_Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE54011-B1AF-441C-B044-4B2BA4F5D40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24CD14D-58F4-4A13-A2DC-303D6BEEF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="156">
   <si>
     <t>TC_01</t>
   </si>
@@ -472,6 +472,132 @@
   </si>
   <si>
     <t>KaiKaci Event Test Cases</t>
+  </si>
+  <si>
+    <t>TC_05_01</t>
+  </si>
+  <si>
+    <t>Organizer creates event with valid data</t>
+  </si>
+  <si>
+    <t>Tester is logged in as an organizer and on the Create Event page.</t>
+  </si>
+  <si>
+    <t>1. Enter a valid Image URL.
+2. Fill Title and Description fields.
+3. Add two open‑ended questions.
+4. Click 'Create Event'.</t>
+  </si>
+  <si>
+    <t>1. Event is saved successfully.
+2. Toast/banner 'Event created' is shown.
+3. User is redirected to the new event page.
+4. Event card appears on the landing page with status 'Open'.</t>
+  </si>
+  <si>
+    <t>TC_05_02</t>
+  </si>
+  <si>
+    <t>Creation fails when required fields are empty</t>
+  </si>
+  <si>
+    <t>Tester is logged in and on the Create Event page.</t>
+  </si>
+  <si>
+    <t>1. Leave the Title field blank.
+2. Fill other fields normally.
+3. Click 'Create Event'.</t>
+  </si>
+  <si>
+    <t>1. Event is NOT created.
+2. Inline validation 'Title is required' appears below the field.
+3. Form remains open for correction.</t>
+  </si>
+  <si>
+    <t>TC_05_03</t>
+  </si>
+  <si>
+    <t>Image URL is validated</t>
+  </si>
+  <si>
+    <t>Tester is on the Create Event page.</t>
+  </si>
+  <si>
+    <t>1. Enter 'not_a_url' in the Image URL field.
+2. Fill other required fields correctly.
+3. Click 'Create Event'.</t>
+  </si>
+  <si>
+    <t>1. Validation error 'Invalid URL format' is displayed.
+2. Event is not created until a valid URL is provided.</t>
+  </si>
+  <si>
+    <t>TC_05_04</t>
+  </si>
+  <si>
+    <t>Organizer updates event description and image</t>
+  </si>
+  <si>
+    <t>Tester is logged in as the event's organizer and on the Manage Event page.</t>
+  </si>
+  <si>
+    <t>1. Replace current Description with new text.
+2. Paste a new valid Image URL.
+3. Click 'Update Event'.</t>
+  </si>
+  <si>
+    <t>1. Update succeeds and success banner appears.
+2. Event page shows the new description and image.
+3. Landing-page card displays the updated image.</t>
+  </si>
+  <si>
+    <t>TC_05_05</t>
+  </si>
+  <si>
+    <t>Questions are read‑only during edit</t>
+  </si>
+  <si>
+    <t>Tester is on the Manage Event page.</t>
+  </si>
+  <si>
+    <t>1. Locate the Questions section.
+2. Attempt to edit existing question text.</t>
+  </si>
+  <si>
+    <t>1. Question inputs are disabled (read‑only) or no edit icon is present.
+2. User cannot modify questions after event creation.</t>
+  </si>
+  <si>
+    <t>TC_05_06</t>
+  </si>
+  <si>
+    <t>Organizer deletes event after confirmation</t>
+  </si>
+  <si>
+    <t>1. Click 'Delete Event'.
+2. Confirm deletion in the modal dialog.</t>
+  </si>
+  <si>
+    <t>1. Event is removed from database.
+2. User is redirected to 'Manage My Events' list.
+3. Event card no longer appears on landing page.</t>
+  </si>
+  <si>
+    <t>TC_05_07</t>
+  </si>
+  <si>
+    <t>Delete cancellation keeps event intact</t>
+  </si>
+  <si>
+    <t>1. Click 'Delete Event'.
+2. Click 'Cancel' in the confirmation dialog.</t>
+  </si>
+  <si>
+    <t>1. Dialog closes with no action.
+2. Event remains on Manage Event page and landing page.</t>
+  </si>
+  <si>
+    <t>KaiKaci Event Create/Edit Test Cases</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -1905,7 +2031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="15" outlineLevel="1">
+    <row r="65" spans="1:7" ht="15" outlineLevel="1">
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -1913,7 +2039,7 @@
       <c r="F65" s="19"/>
       <c r="G65" s="23"/>
     </row>
-    <row r="66" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="66" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B66" s="10" t="s">
         <v>2</v>
       </c>
@@ -1933,7 +2059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="99.75" outlineLevel="1">
+    <row r="67" spans="1:7" ht="99.75" outlineLevel="1">
       <c r="B67" s="22" t="s">
         <v>100</v>
       </c>
@@ -1953,7 +2079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="15" outlineLevel="1">
+    <row r="68" spans="1:7" ht="15" outlineLevel="1">
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
@@ -1961,7 +2087,7 @@
       <c r="F68" s="19"/>
       <c r="G68" s="23"/>
     </row>
-    <row r="69" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="69" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B69" s="10" t="s">
         <v>2</v>
       </c>
@@ -1981,7 +2107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="114" outlineLevel="1">
+    <row r="70" spans="1:7" ht="114" outlineLevel="1">
       <c r="B70" s="22" t="s">
         <v>105</v>
       </c>
@@ -2001,7 +2127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="2:7" ht="15" outlineLevel="1">
+    <row r="71" spans="1:7" ht="15" outlineLevel="1">
       <c r="B71" s="19"/>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -2009,7 +2135,7 @@
       <c r="F71" s="19"/>
       <c r="G71" s="23"/>
     </row>
-    <row r="72" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="72" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B72" s="10" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="2:7" ht="99.75" outlineLevel="1">
+    <row r="73" spans="1:7" ht="99.75" outlineLevel="1">
       <c r="B73" s="22" t="s">
         <v>110</v>
       </c>
@@ -2049,7 +2175,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="2:7" ht="15" outlineLevel="1">
+    <row r="74" spans="1:7" ht="15" outlineLevel="1">
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
       <c r="D74" s="19"/>
@@ -2057,7 +2183,7 @@
       <c r="F74" s="19"/>
       <c r="G74" s="23"/>
     </row>
-    <row r="75" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="75" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B75" s="10" t="s">
         <v>2</v>
       </c>
@@ -2077,7 +2203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="2:7" ht="114" outlineLevel="1">
+    <row r="76" spans="1:7" ht="114" outlineLevel="1">
       <c r="B76" s="22" t="s">
         <v>115</v>
       </c>
@@ -2097,10 +2223,351 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="2:7" outlineLevel="1"/>
-    <row r="78" spans="2:7" outlineLevel="1"/>
+    <row r="77" spans="1:7" outlineLevel="1"/>
+    <row r="78" spans="1:7" outlineLevel="1"/>
+    <row r="80" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A80" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G80" s="27"/>
+    </row>
+    <row r="81" spans="2:7" outlineLevel="1"/>
+    <row r="82" spans="2:7" outlineLevel="1"/>
+    <row r="83" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B83" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="120" outlineLevel="1">
+      <c r="B84" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G84" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B85" s="28"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="28"/>
+    </row>
+    <row r="86" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B86" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F86" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G86" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" ht="90" outlineLevel="1">
+      <c r="B87" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G87" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B88" s="28"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="28"/>
+    </row>
+    <row r="89" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B89" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G89" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" ht="75" outlineLevel="1">
+      <c r="B90" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G90" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B91" s="28"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="28"/>
+    </row>
+    <row r="92" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B92" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G92" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="90" outlineLevel="1">
+      <c r="B93" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G93" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B94" s="28"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="28"/>
+    </row>
+    <row r="95" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B95" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F95" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="75" outlineLevel="1">
+      <c r="B96" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F96" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B97" s="28"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="28"/>
+    </row>
+    <row r="98" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B98" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" ht="90" outlineLevel="1">
+      <c r="B99" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G99" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B100" s="28"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="28"/>
+    </row>
+    <row r="101" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B101" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G101" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="60" outlineLevel="1">
+      <c r="B102" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C102" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="F102" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G102" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" outlineLevel="1"/>
+    <row r="104" spans="2:7" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding test case group for Volunteer Management test cases
</commit_message>
<xml_diff>
--- a/KaiKaci_Manual_Test_Cases.xlsx
+++ b/KaiKaci_Manual_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\FinalSoftware\KIU_Volunteer_Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24CD14D-58F4-4A13-A2DC-303D6BEEF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C677C6-09F8-4428-8064-FF10FBCCCB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="184">
   <si>
     <t>TC_01</t>
   </si>
@@ -598,6 +598,104 @@
   </si>
   <si>
     <t>KaiKaci Event Create/Edit Test Cases</t>
+  </si>
+  <si>
+    <t>TC_06_01</t>
+  </si>
+  <si>
+    <t>Volunteer list displays correct info</t>
+  </si>
+  <si>
+    <t>Organizer is logged in and on the Manage Volunteers page for an event with at least three volunteer submissions.</t>
+  </si>
+  <si>
+    <t>1. Observe the volunteer cards grid/list.</t>
+  </si>
+  <si>
+    <t>1. Each card shows Name, Age, Sex, Email, and Status (default 'Pending').
+2. Total count of volunteers is displayed near the page title.</t>
+  </si>
+  <si>
+    <t>TC_06_02</t>
+  </si>
+  <si>
+    <t>Volunteer details modal shows full application</t>
+  </si>
+  <si>
+    <t>Organizer is on Manage Volunteers page.</t>
+  </si>
+  <si>
+    <t>1. Click a volunteer card.
+2. Observe the modal/dialog that opens.</t>
+  </si>
+  <si>
+    <t>1. Modal appears containing all question‑answer pairs submitted by the volunteer.
+2. Accept, Deny, and Close buttons are visible at the bottom.</t>
+  </si>
+  <si>
+    <t>TC_06_03</t>
+  </si>
+  <si>
+    <t>Organizer accepts an individual volunteer</t>
+  </si>
+  <si>
+    <t>Volunteer status = Pending. Organizer is viewing the volunteer details modal.</t>
+  </si>
+  <si>
+    <t>1. Click 'Accept'.
+2. Confirm action if prompted.</t>
+  </si>
+  <si>
+    <t>1. Modal closes.
+2. Volunteer card status changes to 'Accepted' (green badge).
+3. Accept/Deny buttons are disabled or replaced with static status in the card.</t>
+  </si>
+  <si>
+    <t>TC_06_04</t>
+  </si>
+  <si>
+    <t>Organizer denies an individual volunteer</t>
+  </si>
+  <si>
+    <t>Volunteer status = Pending.</t>
+  </si>
+  <si>
+    <t>1. Open volunteer details modal.
+2. Click 'Deny'.
+3. Confirm action.</t>
+  </si>
+  <si>
+    <t>1. Modal closes.
+2. Volunteer card status changes to 'Denied' (red badge).
+3. Volunteer cannot be accepted afterward (button disabled).</t>
+  </si>
+  <si>
+    <t>TC_06_05</t>
+  </si>
+  <si>
+    <t>Bulk accept selected volunteers</t>
+  </si>
+  <si>
+    <t>At least two volunteers have status = Pending.</t>
+  </si>
+  <si>
+    <t>1. Select checkboxes on two volunteer cards.
+2. Click 'Bulk Accept' toolbar button.
+3. Confirm action.</t>
+  </si>
+  <si>
+    <t>1. Both selected volunteers change status to 'Accepted'.
+2. Success toast '2 volunteers accepted' appears.
+3. Bulk action buttons become disabled if no rows are selected.</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>KaiKaci Volunteer Mgmt Test Cases</t>
   </si>
 </sst>
 </file>
@@ -777,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -855,6 +953,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1159,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -2227,7 +2334,7 @@
     <row r="78" spans="1:7" outlineLevel="1"/>
     <row r="80" spans="1:7" s="1" customFormat="1" ht="15.75">
       <c r="A80" s="27" t="s">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="B80" s="18" t="s">
         <v>155</v>
@@ -2468,7 +2575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="2:7" ht="15" outlineLevel="1">
+    <row r="97" spans="1:7" ht="15" outlineLevel="1">
       <c r="B97" s="28"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
@@ -2476,7 +2583,7 @@
       <c r="F97" s="12"/>
       <c r="G97" s="28"/>
     </row>
-    <row r="98" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="98" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B98" s="25" t="s">
         <v>2</v>
       </c>
@@ -2496,7 +2603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="90" outlineLevel="1">
+    <row r="99" spans="1:7" ht="90" outlineLevel="1">
       <c r="B99" s="17" t="s">
         <v>147</v>
       </c>
@@ -2516,7 +2623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="15" outlineLevel="1">
+    <row r="100" spans="1:7" ht="15" outlineLevel="1">
       <c r="B100" s="28"/>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
@@ -2524,7 +2631,7 @@
       <c r="F100" s="12"/>
       <c r="G100" s="28"/>
     </row>
-    <row r="101" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="101" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B101" s="25" t="s">
         <v>2</v>
       </c>
@@ -2544,7 +2651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="2:7" ht="60" outlineLevel="1">
+    <row r="102" spans="1:7" ht="60" outlineLevel="1">
       <c r="B102" s="17" t="s">
         <v>151</v>
       </c>
@@ -2564,8 +2671,260 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="2:7" outlineLevel="1"/>
-    <row r="104" spans="2:7" outlineLevel="1"/>
+    <row r="103" spans="1:7" outlineLevel="1"/>
+    <row r="104" spans="1:7" outlineLevel="1"/>
+    <row r="106" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A106" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G106" s="27"/>
+    </row>
+    <row r="107" spans="1:7" outlineLevel="1"/>
+    <row r="108" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B108" s="31"/>
+      <c r="C108" s="31"/>
+      <c r="D108" s="31"/>
+      <c r="E108" s="31"/>
+      <c r="F108" s="31"/>
+      <c r="G108" s="31"/>
+    </row>
+    <row r="109" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B109" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F109" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G109" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="90" outlineLevel="1">
+      <c r="B110" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G110" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B111" s="28"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="28"/>
+    </row>
+    <row r="112" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B112" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C112" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D112" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E112" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G112" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" ht="90" outlineLevel="1">
+      <c r="B113" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F113" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G113" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B114" s="28"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="28"/>
+    </row>
+    <row r="115" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B115" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C115" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D115" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E115" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F115" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G115" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" ht="105" outlineLevel="1">
+      <c r="B116" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C116" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F116" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G116" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B117" s="28"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+      <c r="G117" s="28"/>
+    </row>
+    <row r="118" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B118" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C118" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E118" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F118" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G118" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" ht="105" outlineLevel="1">
+      <c r="B119" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F119" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G119" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B120" s="28"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="28"/>
+    </row>
+    <row r="121" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B121" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D121" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E121" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F121" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G121" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" ht="105" outlineLevel="1">
+      <c r="B122" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F122" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="G122" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" outlineLevel="1"/>
+    <row r="124" spans="2:7" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding test case group for My Submissions test cases
</commit_message>
<xml_diff>
--- a/KaiKaci_Manual_Test_Cases.xlsx
+++ b/KaiKaci_Manual_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\FinalSoftware\KIU_Volunteer_Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C677C6-09F8-4428-8064-FF10FBCCCB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8381D66B-8015-40FA-B5A7-929A56F70D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="211">
   <si>
     <t>TC_01</t>
   </si>
@@ -696,6 +696,99 @@
   </si>
   <si>
     <t>KaiKaci Volunteer Mgmt Test Cases</t>
+  </si>
+  <si>
+    <t>TC_07_01</t>
+  </si>
+  <si>
+    <t>Submissions list shows correct status badges</t>
+  </si>
+  <si>
+    <t>Tester is logged in as a volunteer with at least three submissions: Pending, Accepted, and Denied.</t>
+  </si>
+  <si>
+    <t>1. Navigate to 'My Submissions' page via account menu.
+2. Observe the event cards list.</t>
+  </si>
+  <si>
+    <t>1. Cards display event Title, Date, and Location.
+2. Each card shows a status badge: 'Pending' (yellow), 'Accepted' (green), 'Denied' (red).
+3. Total submissions count displays near the page title.</t>
+  </si>
+  <si>
+    <t>TC_07_02</t>
+  </si>
+  <si>
+    <t>Volunteer cancels a Pending submission</t>
+  </si>
+  <si>
+    <t>Tester has a submission with status = Pending and is on My Submissions page.</t>
+  </si>
+  <si>
+    <t>1. Locate the Pending submission card.
+2. Click 'Cancel Request'.
+3. Confirm cancellation in modal.</t>
+  </si>
+  <si>
+    <t>1. Card status changes to 'Withdrawn' (grey badge).
+2. Cancel button disappears or is disabled.
+3. Success toast/banner confirms cancellation.</t>
+  </si>
+  <si>
+    <t>TC_07_03</t>
+  </si>
+  <si>
+    <t>Cancel button disabled for Accepted or Denied submissions</t>
+  </si>
+  <si>
+    <t>Tester has submissions with status Accepted and Denied.</t>
+  </si>
+  <si>
+    <t>1. Locate Accepted submission card.
+2. Observe the card buttons.
+3. Repeat for Denied submission.</t>
+  </si>
+  <si>
+    <t>1. 'Cancel Request' button is hidden or disabled for Accepted and Denied statuses.
+2. User cannot trigger cancellation for these submissions.</t>
+  </si>
+  <si>
+    <t>TC_07_04</t>
+  </si>
+  <si>
+    <t>Clicking a submission card opens its Event page</t>
+  </si>
+  <si>
+    <t>Tester is on My Submissions page.</t>
+  </si>
+  <si>
+    <t>1. Click any submission card (regardless of status).</t>
+  </si>
+  <si>
+    <t>1. Browser navigates to the corresponding Event Details page.
+2. Event page loads successfully with correct information.</t>
+  </si>
+  <si>
+    <t>TC_07_05</t>
+  </si>
+  <si>
+    <t>Empty state shown when no submissions exist</t>
+  </si>
+  <si>
+    <t>Tester is logged in but has no submissions in database.</t>
+  </si>
+  <si>
+    <t>1. Navigate to My Submissions page.</t>
+  </si>
+  <si>
+    <t>1. Friendly empty‑state banner is shown (e.g., 'You haven’t applied to any events yet').
+2. CTA button 'Browse Events' routes back to landing page.</t>
+  </si>
+  <si>
+    <t>TC_07</t>
+  </si>
+  <si>
+    <t>KaiKaci My Submissions Test Cases</t>
   </si>
 </sst>
 </file>
@@ -1266,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F130" sqref="F130"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -2759,7 +2852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="2:7" ht="90" outlineLevel="1">
+    <row r="113" spans="1:7" ht="90" outlineLevel="1">
       <c r="B113" s="17" t="s">
         <v>161</v>
       </c>
@@ -2779,7 +2872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" spans="2:7" ht="15" outlineLevel="1">
+    <row r="114" spans="1:7" ht="15" outlineLevel="1">
       <c r="B114" s="28"/>
       <c r="C114" s="12"/>
       <c r="D114" s="12"/>
@@ -2787,7 +2880,7 @@
       <c r="F114" s="12"/>
       <c r="G114" s="28"/>
     </row>
-    <row r="115" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="115" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B115" s="32" t="s">
         <v>2</v>
       </c>
@@ -2807,7 +2900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="2:7" ht="105" outlineLevel="1">
+    <row r="116" spans="1:7" ht="105" outlineLevel="1">
       <c r="B116" s="17" t="s">
         <v>166</v>
       </c>
@@ -2827,7 +2920,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="2:7" ht="15" outlineLevel="1">
+    <row r="117" spans="1:7" ht="15" outlineLevel="1">
       <c r="B117" s="28"/>
       <c r="C117" s="12"/>
       <c r="D117" s="12"/>
@@ -2835,7 +2928,7 @@
       <c r="F117" s="12"/>
       <c r="G117" s="28"/>
     </row>
-    <row r="118" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="118" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B118" s="32" t="s">
         <v>2</v>
       </c>
@@ -2855,7 +2948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="2:7" ht="105" outlineLevel="1">
+    <row r="119" spans="1:7" ht="105" outlineLevel="1">
       <c r="B119" s="17" t="s">
         <v>171</v>
       </c>
@@ -2875,7 +2968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="15" outlineLevel="1">
+    <row r="120" spans="1:7" ht="15" outlineLevel="1">
       <c r="B120" s="28"/>
       <c r="C120" s="12"/>
       <c r="D120" s="12"/>
@@ -2883,7 +2976,7 @@
       <c r="F120" s="12"/>
       <c r="G120" s="28"/>
     </row>
-    <row r="121" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="121" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B121" s="32" t="s">
         <v>2</v>
       </c>
@@ -2903,7 +2996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="105" outlineLevel="1">
+    <row r="122" spans="1:7" ht="105" outlineLevel="1">
       <c r="B122" s="17" t="s">
         <v>176</v>
       </c>
@@ -2923,8 +3016,253 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="2:7" outlineLevel="1"/>
-    <row r="124" spans="2:7" outlineLevel="1"/>
+    <row r="123" spans="1:7" outlineLevel="1"/>
+    <row r="124" spans="1:7" outlineLevel="1"/>
+    <row r="126" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A126" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B126" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G126" s="27"/>
+    </row>
+    <row r="127" spans="1:7" outlineLevel="1"/>
+    <row r="128" spans="1:7" outlineLevel="1"/>
+    <row r="129" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B129" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D129" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E129" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F129" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G129" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" ht="120" outlineLevel="1">
+      <c r="B130" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E130" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F130" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G130" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B131" s="28"/>
+      <c r="C131" s="12"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12"/>
+      <c r="G131" s="28"/>
+    </row>
+    <row r="132" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B132" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C132" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D132" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E132" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G132" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" ht="90" outlineLevel="1">
+      <c r="B133" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C133" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E133" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F133" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G133" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B134" s="28"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
+      <c r="G134" s="28"/>
+    </row>
+    <row r="135" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B135" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E135" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F135" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G135" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" ht="90" outlineLevel="1">
+      <c r="B136" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C136" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E136" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F136" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G136" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B137" s="28"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
+      <c r="G137" s="28"/>
+    </row>
+    <row r="138" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B138" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D138" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E138" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F138" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G138" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" ht="75" outlineLevel="1">
+      <c r="B139" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C139" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D139" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E139" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F139" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="G139" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B140" s="28"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="28"/>
+    </row>
+    <row r="141" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B141" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D141" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E141" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F141" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G141" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" ht="75" outlineLevel="1">
+      <c r="B142" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D142" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E142" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="F142" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G142" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" outlineLevel="1"/>
+    <row r="144" spans="2:7" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding test case group for Nav/Footer test cases
</commit_message>
<xml_diff>
--- a/KaiKaci_Manual_Test_Cases.xlsx
+++ b/KaiKaci_Manual_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\FinalSoftware\KIU_Volunteer_Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8381D66B-8015-40FA-B5A7-929A56F70D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353A1BC7-D26B-4E2C-A311-B56140847C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="236">
   <si>
     <t>TC_01</t>
   </si>
@@ -789,6 +789,92 @@
   </si>
   <si>
     <t>KaiKaci My Submissions Test Cases</t>
+  </si>
+  <si>
+    <t>TC_08_01</t>
+  </si>
+  <si>
+    <t>Logo + name link navigates to Landing page</t>
+  </si>
+  <si>
+    <t>Tester is on any non‑landing page (e.g., Event Details).</t>
+  </si>
+  <si>
+    <t>1. Click the KaiKaci logo/name in the nav bar.</t>
+  </si>
+  <si>
+    <t>1. Browser navigates to the Landing page URL.
+2. Landing page content loads without errors.</t>
+  </si>
+  <si>
+    <t>TC_08_02</t>
+  </si>
+  <si>
+    <t>Account dropdown shows correct menu items</t>
+  </si>
+  <si>
+    <t>1. Hover over the Account name in the nav bar.
+2. Observe dropdown items.</t>
+  </si>
+  <si>
+    <t>1. Dropdown lists: 'My Submissions', 'Manage My Events', 'Logout'.
+2. Items are clickable (cursor pointer).</t>
+  </si>
+  <si>
+    <t>TC_08_03</t>
+  </si>
+  <si>
+    <t>Account dropdown links route correctly</t>
+  </si>
+  <si>
+    <t>Prerequisite of TC_08_02 met.</t>
+  </si>
+  <si>
+    <t>1. Click 'My Submissions'.
+2. Verify navigation.
+3. Hover over Account name again.
+4. Click 'Manage My Events'.</t>
+  </si>
+  <si>
+    <t>1. Step 1 → My Submissions page opens.
+2. Step 3‑4 → Manage My Events page opens.
+3. Browser history contains both navigations.</t>
+  </si>
+  <si>
+    <t>TC_08_04</t>
+  </si>
+  <si>
+    <t>Footer is visible and sticky at bottom</t>
+  </si>
+  <si>
+    <t>Tester is on the landing page and window height &gt; content height.</t>
+  </si>
+  <si>
+    <t>1. Scroll to page bottom.</t>
+  </si>
+  <si>
+    <t>1. Footer section is visible.
+2. Footer remains at bottom of viewport on short pages (sticky).</t>
+  </si>
+  <si>
+    <t>TC_08_05</t>
+  </si>
+  <si>
+    <t>Footer external links open in new tab</t>
+  </si>
+  <si>
+    <t>1. In the footer, Ctrl+Click (or middle‑click) the first external link (e.g., GitHub repo).
+2. Observe browser behavior.</t>
+  </si>
+  <si>
+    <t>1. Link opens in a new browser tab.
+2. Original tab remains on landing page.</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>KaiKaci Nav/Footer Test Cases</t>
   </si>
 </sst>
 </file>
@@ -1359,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F167" sqref="F167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -3263,6 +3349,251 @@
     </row>
     <row r="143" spans="2:7" outlineLevel="1"/>
     <row r="144" spans="2:7" outlineLevel="1"/>
+    <row r="146" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A146" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="B146" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G146" s="27"/>
+    </row>
+    <row r="147" spans="1:7" outlineLevel="1"/>
+    <row r="148" spans="1:7" outlineLevel="1"/>
+    <row r="149" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B149" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D149" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E149" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F149" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G149" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="60" outlineLevel="1">
+      <c r="B150" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D150" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E150" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="F150" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="G150" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B151" s="28"/>
+      <c r="C151" s="12"/>
+      <c r="D151" s="12"/>
+      <c r="E151" s="12"/>
+      <c r="F151" s="12"/>
+      <c r="G151" s="28"/>
+    </row>
+    <row r="152" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B152" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D152" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E152" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F152" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G152" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="75" outlineLevel="1">
+      <c r="B153" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C153" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D153" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E153" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F153" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="G153" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B154" s="28"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="12"/>
+      <c r="E154" s="12"/>
+      <c r="F154" s="12"/>
+      <c r="G154" s="28"/>
+    </row>
+    <row r="155" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B155" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C155" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D155" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E155" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F155" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G155" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="90" outlineLevel="1">
+      <c r="B156" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D156" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E156" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="F156" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="G156" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B157" s="28"/>
+      <c r="C157" s="12"/>
+      <c r="D157" s="12"/>
+      <c r="E157" s="12"/>
+      <c r="F157" s="12"/>
+      <c r="G157" s="28"/>
+    </row>
+    <row r="158" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B158" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C158" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D158" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E158" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G158" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="60" outlineLevel="1">
+      <c r="B159" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C159" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E159" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F159" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G159" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B160" s="28"/>
+      <c r="C160" s="12"/>
+      <c r="D160" s="12"/>
+      <c r="E160" s="12"/>
+      <c r="F160" s="12"/>
+      <c r="G160" s="28"/>
+    </row>
+    <row r="161" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B161" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D161" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E161" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F161" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G161" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" ht="60" outlineLevel="1">
+      <c r="B162" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C162" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E162" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F162" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="G162" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" outlineLevel="1"/>
+    <row r="164" spans="2:7" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding test case group for Responsiveness test cases
</commit_message>
<xml_diff>
--- a/KaiKaci_Manual_Test_Cases.xlsx
+++ b/KaiKaci_Manual_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kakha\Desktop\FinalSoftware\KIU_Volunteer_Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353A1BC7-D26B-4E2C-A311-B56140847C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071E582E-970D-4A01-8373-8A0DC6A8C998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="263">
   <si>
     <t>TC_01</t>
   </si>
@@ -875,6 +875,98 @@
   </si>
   <si>
     <t>KaiKaci Nav/Footer Test Cases</t>
+  </si>
+  <si>
+    <t>TC_09_01</t>
+  </si>
+  <si>
+    <t>Mobile nav collapses into hamburger menu (&lt;768 px)</t>
+  </si>
+  <si>
+    <t>Browser viewport is resized to 375 × 812 (iPhone X). Tester is on landing page.</t>
+  </si>
+  <si>
+    <t>1. Observe the nav bar.
+2. Click the hamburger icon.</t>
+  </si>
+  <si>
+    <t>1. Logo remains visible; search and account items are hidden behind hamburger.
+2. Menu slides in or drops down listing Search, Login/Account.
+3. Clicking outside the menu closes it.</t>
+  </si>
+  <si>
+    <t>TC_09_02</t>
+  </si>
+  <si>
+    <t>Event cards wrap to single‑column on mobile</t>
+  </si>
+  <si>
+    <t>Viewport set to 375 × 812. Landing page has ≥3 event cards.</t>
+  </si>
+  <si>
+    <t>1. Scroll through the event grid.</t>
+  </si>
+  <si>
+    <t>1. Event cards display one per row (full‑width).
+2. Card content remains readable; text does not overflow.
+3. No horizontal scrolling appears.</t>
+  </si>
+  <si>
+    <t>TC_09_03</t>
+  </si>
+  <si>
+    <t>Volunteer registration form fits on small screens</t>
+  </si>
+  <si>
+    <t>Tester is on Event page (open). Viewport set to 375 × 812 and logged in.</t>
+  </si>
+  <si>
+    <t>1. Tap 'Register as Volunteer'.
+2. Observe the question modal.</t>
+  </si>
+  <si>
+    <t>1. Modal width adapts to 90‑95 % of viewport.
+2. Inputs fit without horizontal scroll.
+3. Submit / Cancel buttons are fully visible.</t>
+  </si>
+  <si>
+    <t>TC_09_04</t>
+  </si>
+  <si>
+    <t>Tablet (768‑1024 px) shows two‑column card layout</t>
+  </si>
+  <si>
+    <t>Viewport set to 834 × 1112 (iPad Pro portrait).</t>
+  </si>
+  <si>
+    <t>1. Refresh landing page.</t>
+  </si>
+  <si>
+    <t>1. Event grid shows two cards per row.
+2. Card spacing is even; no overlap.</t>
+  </si>
+  <si>
+    <t>TC_09_05</t>
+  </si>
+  <si>
+    <t>Footer stacks vertically on mobile</t>
+  </si>
+  <si>
+    <t>Viewport set to 375 × 812. Tester is on landing page.</t>
+  </si>
+  <si>
+    <t>1. Scroll to footer area.</t>
+  </si>
+  <si>
+    <t>1. Footer columns stack vertically (logo, links, copyright).
+2. Padding keeps items readable.
+3. No text overlaps or truncates.</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>KaiKaci Responsiveness Test Cases</t>
   </si>
 </sst>
 </file>
@@ -1445,10 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F167" sqref="F167"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -3552,7 +3644,7 @@
       <c r="F160" s="12"/>
       <c r="G160" s="28"/>
     </row>
-    <row r="161" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+    <row r="161" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="B161" s="32" t="s">
         <v>2</v>
       </c>
@@ -3572,7 +3664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="2:7" ht="60" outlineLevel="1">
+    <row r="162" spans="1:7" ht="60" outlineLevel="1">
       <c r="B162" s="17" t="s">
         <v>230</v>
       </c>
@@ -3592,8 +3684,253 @@
         <v>30</v>
       </c>
     </row>
-    <row r="163" spans="2:7" outlineLevel="1"/>
-    <row r="164" spans="2:7" outlineLevel="1"/>
+    <row r="163" spans="1:7" outlineLevel="1"/>
+    <row r="164" spans="1:7" outlineLevel="1"/>
+    <row r="166" spans="1:7" s="1" customFormat="1" ht="15.75">
+      <c r="A166" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B166" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="G166" s="27"/>
+    </row>
+    <row r="167" spans="1:7" outlineLevel="1"/>
+    <row r="168" spans="1:7" outlineLevel="1"/>
+    <row r="169" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B169" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C169" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D169" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E169" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F169" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G169" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="120" outlineLevel="1">
+      <c r="B170" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C170" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D170" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E170" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="F170" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G170" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B171" s="28"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="12"/>
+      <c r="E171" s="12"/>
+      <c r="F171" s="12"/>
+      <c r="G171" s="28"/>
+    </row>
+    <row r="172" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B172" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C172" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E172" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F172" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G172" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="105" outlineLevel="1">
+      <c r="B173" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C173" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D173" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="E173" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F173" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G173" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="15" outlineLevel="1">
+      <c r="B174" s="28"/>
+      <c r="C174" s="12"/>
+      <c r="D174" s="12"/>
+      <c r="E174" s="12"/>
+      <c r="F174" s="12"/>
+      <c r="G174" s="28"/>
+    </row>
+    <row r="175" spans="1:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B175" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C175" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D175" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E175" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F175" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G175" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="90" outlineLevel="1">
+      <c r="B176" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C176" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D176" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E176" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="F176" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="G176" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B177" s="28"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="12"/>
+      <c r="E177" s="12"/>
+      <c r="F177" s="12"/>
+      <c r="G177" s="28"/>
+    </row>
+    <row r="178" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B178" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C178" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E178" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F178" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G178" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" ht="75" outlineLevel="1">
+      <c r="B179" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C179" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="D179" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E179" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F179" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G179" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" ht="15" outlineLevel="1">
+      <c r="B180" s="28"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
+      <c r="F180" s="12"/>
+      <c r="G180" s="28"/>
+    </row>
+    <row r="181" spans="2:7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="B181" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C181" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D181" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E181" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F181" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G181" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7" ht="105" outlineLevel="1">
+      <c r="B182" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="C182" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D182" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="E182" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="F182" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G182" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" outlineLevel="1"/>
+    <row r="184" spans="2:7" outlineLevel="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>